<commit_message>
Added market cap and shares outstanding
</commit_message>
<xml_diff>
--- a/data/cds_spread.xlsx
+++ b/data/cds_spread.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="3">
   <si>
     <t>Instrument</t>
   </si>
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1567"/>
+  <dimension ref="A1:C1829"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17620,6 +17620,2888 @@
         <v>93.03</v>
       </c>
     </row>
+    <row r="1568" spans="1:3">
+      <c r="A1568" s="1">
+        <v>1566</v>
+      </c>
+      <c r="B1568" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1568">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:3">
+      <c r="A1569" s="1">
+        <v>1567</v>
+      </c>
+      <c r="B1569" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1569">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:3">
+      <c r="A1570" s="1">
+        <v>1568</v>
+      </c>
+      <c r="B1570" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1570">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:3">
+      <c r="A1571" s="1">
+        <v>1569</v>
+      </c>
+      <c r="B1571" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1571">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:3">
+      <c r="A1572" s="1">
+        <v>1570</v>
+      </c>
+      <c r="B1572" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1572">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:3">
+      <c r="A1573" s="1">
+        <v>1571</v>
+      </c>
+      <c r="B1573" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1573">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:3">
+      <c r="A1574" s="1">
+        <v>1572</v>
+      </c>
+      <c r="B1574" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1574">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:3">
+      <c r="A1575" s="1">
+        <v>1573</v>
+      </c>
+      <c r="B1575" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1575">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:3">
+      <c r="A1576" s="1">
+        <v>1574</v>
+      </c>
+      <c r="B1576" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1576">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:3">
+      <c r="A1577" s="1">
+        <v>1575</v>
+      </c>
+      <c r="B1577" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1577">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:3">
+      <c r="A1578" s="1">
+        <v>1576</v>
+      </c>
+      <c r="B1578" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1578">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:3">
+      <c r="A1579" s="1">
+        <v>1577</v>
+      </c>
+      <c r="B1579" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1579">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:3">
+      <c r="A1580" s="1">
+        <v>1578</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1580">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:3">
+      <c r="A1581" s="1">
+        <v>1579</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1581">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:3">
+      <c r="A1582" s="1">
+        <v>1580</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1582">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:3">
+      <c r="A1583" s="1">
+        <v>1581</v>
+      </c>
+      <c r="B1583" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1583">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:3">
+      <c r="A1584" s="1">
+        <v>1582</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1584">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:3">
+      <c r="A1585" s="1">
+        <v>1583</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1585">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:3">
+      <c r="A1586" s="1">
+        <v>1584</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1586">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:3">
+      <c r="A1587" s="1">
+        <v>1585</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1587">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:3">
+      <c r="A1588" s="1">
+        <v>1586</v>
+      </c>
+      <c r="B1588" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1588">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:3">
+      <c r="A1589" s="1">
+        <v>1587</v>
+      </c>
+      <c r="B1589" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1589">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:3">
+      <c r="A1590" s="1">
+        <v>1588</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1590">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:3">
+      <c r="A1591" s="1">
+        <v>1589</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1591">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:3">
+      <c r="A1592" s="1">
+        <v>1590</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1592">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:3">
+      <c r="A1593" s="1">
+        <v>1591</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1593">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:3">
+      <c r="A1594" s="1">
+        <v>1592</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1594">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:3">
+      <c r="A1595" s="1">
+        <v>1593</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1595">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:3">
+      <c r="A1596" s="1">
+        <v>1594</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1596">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:3">
+      <c r="A1597" s="1">
+        <v>1595</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1597">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:3">
+      <c r="A1598" s="1">
+        <v>1596</v>
+      </c>
+      <c r="B1598" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1598">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:3">
+      <c r="A1599" s="1">
+        <v>1597</v>
+      </c>
+      <c r="B1599" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1599">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:3">
+      <c r="A1600" s="1">
+        <v>1598</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1600">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:3">
+      <c r="A1601" s="1">
+        <v>1599</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1601">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:3">
+      <c r="A1602" s="1">
+        <v>1600</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1602">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:3">
+      <c r="A1603" s="1">
+        <v>1601</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1603">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:3">
+      <c r="A1604" s="1">
+        <v>1602</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1604">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:3">
+      <c r="A1605" s="1">
+        <v>1603</v>
+      </c>
+      <c r="B1605" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1605">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:3">
+      <c r="A1606" s="1">
+        <v>1604</v>
+      </c>
+      <c r="B1606" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1606">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:3">
+      <c r="A1607" s="1">
+        <v>1605</v>
+      </c>
+      <c r="B1607" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1607">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:3">
+      <c r="A1608" s="1">
+        <v>1606</v>
+      </c>
+      <c r="B1608" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1608">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:3">
+      <c r="A1609" s="1">
+        <v>1607</v>
+      </c>
+      <c r="B1609" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1609">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:3">
+      <c r="A1610" s="1">
+        <v>1608</v>
+      </c>
+      <c r="B1610" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1610">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:3">
+      <c r="A1611" s="1">
+        <v>1609</v>
+      </c>
+      <c r="B1611" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1611">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:3">
+      <c r="A1612" s="1">
+        <v>1610</v>
+      </c>
+      <c r="B1612" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1612">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:3">
+      <c r="A1613" s="1">
+        <v>1611</v>
+      </c>
+      <c r="B1613" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1613">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:3">
+      <c r="A1614" s="1">
+        <v>1612</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1614">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:3">
+      <c r="A1615" s="1">
+        <v>1613</v>
+      </c>
+      <c r="B1615" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1615">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:3">
+      <c r="A1616" s="1">
+        <v>1614</v>
+      </c>
+      <c r="B1616" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1616">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:3">
+      <c r="A1617" s="1">
+        <v>1615</v>
+      </c>
+      <c r="B1617" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1617">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:3">
+      <c r="A1618" s="1">
+        <v>1616</v>
+      </c>
+      <c r="B1618" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1618">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:3">
+      <c r="A1619" s="1">
+        <v>1617</v>
+      </c>
+      <c r="B1619" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1619">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:3">
+      <c r="A1620" s="1">
+        <v>1618</v>
+      </c>
+      <c r="B1620" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1620">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:3">
+      <c r="A1621" s="1">
+        <v>1619</v>
+      </c>
+      <c r="B1621" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1621">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:3">
+      <c r="A1622" s="1">
+        <v>1620</v>
+      </c>
+      <c r="B1622" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1622">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:3">
+      <c r="A1623" s="1">
+        <v>1621</v>
+      </c>
+      <c r="B1623" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1623">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:3">
+      <c r="A1624" s="1">
+        <v>1622</v>
+      </c>
+      <c r="B1624" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1624">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:3">
+      <c r="A1625" s="1">
+        <v>1623</v>
+      </c>
+      <c r="B1625" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1625">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:3">
+      <c r="A1626" s="1">
+        <v>1624</v>
+      </c>
+      <c r="B1626" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1626">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:3">
+      <c r="A1627" s="1">
+        <v>1625</v>
+      </c>
+      <c r="B1627" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1627">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:3">
+      <c r="A1628" s="1">
+        <v>1626</v>
+      </c>
+      <c r="B1628" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1628">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:3">
+      <c r="A1629" s="1">
+        <v>1627</v>
+      </c>
+      <c r="B1629" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1629">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:3">
+      <c r="A1630" s="1">
+        <v>1628</v>
+      </c>
+      <c r="B1630" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1630">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:3">
+      <c r="A1631" s="1">
+        <v>1629</v>
+      </c>
+      <c r="B1631" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1631">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:3">
+      <c r="A1632" s="1">
+        <v>1630</v>
+      </c>
+      <c r="B1632" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1632">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1633" spans="1:3">
+      <c r="A1633" s="1">
+        <v>1631</v>
+      </c>
+      <c r="B1633" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1633">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:3">
+      <c r="A1634" s="1">
+        <v>1632</v>
+      </c>
+      <c r="B1634" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1634">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:3">
+      <c r="A1635" s="1">
+        <v>1633</v>
+      </c>
+      <c r="B1635" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1635">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:3">
+      <c r="A1636" s="1">
+        <v>1634</v>
+      </c>
+      <c r="B1636" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1636">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:3">
+      <c r="A1637" s="1">
+        <v>1635</v>
+      </c>
+      <c r="B1637" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1637">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:3">
+      <c r="A1638" s="1">
+        <v>1636</v>
+      </c>
+      <c r="B1638" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1638">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:3">
+      <c r="A1639" s="1">
+        <v>1637</v>
+      </c>
+      <c r="B1639" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1639">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:3">
+      <c r="A1640" s="1">
+        <v>1638</v>
+      </c>
+      <c r="B1640" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1640">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:3">
+      <c r="A1641" s="1">
+        <v>1639</v>
+      </c>
+      <c r="B1641" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1641">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:3">
+      <c r="A1642" s="1">
+        <v>1640</v>
+      </c>
+      <c r="B1642" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1642">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:3">
+      <c r="A1643" s="1">
+        <v>1641</v>
+      </c>
+      <c r="B1643" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1643">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:3">
+      <c r="A1644" s="1">
+        <v>1642</v>
+      </c>
+      <c r="B1644" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1644">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:3">
+      <c r="A1645" s="1">
+        <v>1643</v>
+      </c>
+      <c r="B1645" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1645">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:3">
+      <c r="A1646" s="1">
+        <v>1644</v>
+      </c>
+      <c r="B1646" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1646">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:3">
+      <c r="A1647" s="1">
+        <v>1645</v>
+      </c>
+      <c r="B1647" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1647">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:3">
+      <c r="A1648" s="1">
+        <v>1646</v>
+      </c>
+      <c r="B1648" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1648">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:3">
+      <c r="A1649" s="1">
+        <v>1647</v>
+      </c>
+      <c r="B1649" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1649">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:3">
+      <c r="A1650" s="1">
+        <v>1648</v>
+      </c>
+      <c r="B1650" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1650">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:3">
+      <c r="A1651" s="1">
+        <v>1649</v>
+      </c>
+      <c r="B1651" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1651">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:3">
+      <c r="A1652" s="1">
+        <v>1650</v>
+      </c>
+      <c r="B1652" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1652">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:3">
+      <c r="A1653" s="1">
+        <v>1651</v>
+      </c>
+      <c r="B1653" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1653">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:3">
+      <c r="A1654" s="1">
+        <v>1652</v>
+      </c>
+      <c r="B1654" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1654">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:3">
+      <c r="A1655" s="1">
+        <v>1653</v>
+      </c>
+      <c r="B1655" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1655">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:3">
+      <c r="A1656" s="1">
+        <v>1654</v>
+      </c>
+      <c r="B1656" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1656">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:3">
+      <c r="A1657" s="1">
+        <v>1655</v>
+      </c>
+      <c r="B1657" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1657">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:3">
+      <c r="A1658" s="1">
+        <v>1656</v>
+      </c>
+      <c r="B1658" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1658">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:3">
+      <c r="A1659" s="1">
+        <v>1657</v>
+      </c>
+      <c r="B1659" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1659">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:3">
+      <c r="A1660" s="1">
+        <v>1658</v>
+      </c>
+      <c r="B1660" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1660">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:3">
+      <c r="A1661" s="1">
+        <v>1659</v>
+      </c>
+      <c r="B1661" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1661">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:3">
+      <c r="A1662" s="1">
+        <v>1660</v>
+      </c>
+      <c r="B1662" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1662">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:3">
+      <c r="A1663" s="1">
+        <v>1661</v>
+      </c>
+      <c r="B1663" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1663">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:3">
+      <c r="A1664" s="1">
+        <v>1662</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1664">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:3">
+      <c r="A1665" s="1">
+        <v>1663</v>
+      </c>
+      <c r="B1665" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1665">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:3">
+      <c r="A1666" s="1">
+        <v>1664</v>
+      </c>
+      <c r="B1666" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1666">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:3">
+      <c r="A1667" s="1">
+        <v>1665</v>
+      </c>
+      <c r="B1667" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1667">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:3">
+      <c r="A1668" s="1">
+        <v>1666</v>
+      </c>
+      <c r="B1668" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1668">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:3">
+      <c r="A1669" s="1">
+        <v>1667</v>
+      </c>
+      <c r="B1669" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1669">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:3">
+      <c r="A1670" s="1">
+        <v>1668</v>
+      </c>
+      <c r="B1670" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1670">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:3">
+      <c r="A1671" s="1">
+        <v>1669</v>
+      </c>
+      <c r="B1671" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1671">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:3">
+      <c r="A1672" s="1">
+        <v>1670</v>
+      </c>
+      <c r="B1672" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1672">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:3">
+      <c r="A1673" s="1">
+        <v>1671</v>
+      </c>
+      <c r="B1673" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1673">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:3">
+      <c r="A1674" s="1">
+        <v>1672</v>
+      </c>
+      <c r="B1674" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1674">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:3">
+      <c r="A1675" s="1">
+        <v>1673</v>
+      </c>
+      <c r="B1675" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1675">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:3">
+      <c r="A1676" s="1">
+        <v>1674</v>
+      </c>
+      <c r="B1676" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1676">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:3">
+      <c r="A1677" s="1">
+        <v>1675</v>
+      </c>
+      <c r="B1677" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1677">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:3">
+      <c r="A1678" s="1">
+        <v>1676</v>
+      </c>
+      <c r="B1678" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1678">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:3">
+      <c r="A1679" s="1">
+        <v>1677</v>
+      </c>
+      <c r="B1679" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1679">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:3">
+      <c r="A1680" s="1">
+        <v>1678</v>
+      </c>
+      <c r="B1680" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1680">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:3">
+      <c r="A1681" s="1">
+        <v>1679</v>
+      </c>
+      <c r="B1681" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1681">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:3">
+      <c r="A1682" s="1">
+        <v>1680</v>
+      </c>
+      <c r="B1682" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1682">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:3">
+      <c r="A1683" s="1">
+        <v>1681</v>
+      </c>
+      <c r="B1683" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1683">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:3">
+      <c r="A1684" s="1">
+        <v>1682</v>
+      </c>
+      <c r="B1684" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1684">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:3">
+      <c r="A1685" s="1">
+        <v>1683</v>
+      </c>
+      <c r="B1685" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1685">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:3">
+      <c r="A1686" s="1">
+        <v>1684</v>
+      </c>
+      <c r="B1686" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1686">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:3">
+      <c r="A1687" s="1">
+        <v>1685</v>
+      </c>
+      <c r="B1687" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1687">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:3">
+      <c r="A1688" s="1">
+        <v>1686</v>
+      </c>
+      <c r="B1688" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1688">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:3">
+      <c r="A1689" s="1">
+        <v>1687</v>
+      </c>
+      <c r="B1689" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1689">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:3">
+      <c r="A1690" s="1">
+        <v>1688</v>
+      </c>
+      <c r="B1690" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1690">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:3">
+      <c r="A1691" s="1">
+        <v>1689</v>
+      </c>
+      <c r="B1691" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1691">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:3">
+      <c r="A1692" s="1">
+        <v>1690</v>
+      </c>
+      <c r="B1692" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1692">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1693" spans="1:3">
+      <c r="A1693" s="1">
+        <v>1691</v>
+      </c>
+      <c r="B1693" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1693">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:3">
+      <c r="A1694" s="1">
+        <v>1692</v>
+      </c>
+      <c r="B1694" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1694">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:3">
+      <c r="A1695" s="1">
+        <v>1693</v>
+      </c>
+      <c r="B1695" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1695">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:3">
+      <c r="A1696" s="1">
+        <v>1694</v>
+      </c>
+      <c r="B1696" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1696">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:3">
+      <c r="A1697" s="1">
+        <v>1695</v>
+      </c>
+      <c r="B1697" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1697">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:3">
+      <c r="A1698" s="1">
+        <v>1696</v>
+      </c>
+      <c r="B1698" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1698">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:3">
+      <c r="A1699" s="1">
+        <v>1697</v>
+      </c>
+      <c r="B1699" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1699">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:3">
+      <c r="A1700" s="1">
+        <v>1698</v>
+      </c>
+      <c r="B1700" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1700">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:3">
+      <c r="A1701" s="1">
+        <v>1699</v>
+      </c>
+      <c r="B1701" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1701">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:3">
+      <c r="A1702" s="1">
+        <v>1700</v>
+      </c>
+      <c r="B1702" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1702">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:3">
+      <c r="A1703" s="1">
+        <v>1701</v>
+      </c>
+      <c r="B1703" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1703">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:3">
+      <c r="A1704" s="1">
+        <v>1702</v>
+      </c>
+      <c r="B1704" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1704">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:3">
+      <c r="A1705" s="1">
+        <v>1703</v>
+      </c>
+      <c r="B1705" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1705">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:3">
+      <c r="A1706" s="1">
+        <v>1704</v>
+      </c>
+      <c r="B1706" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1706">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:3">
+      <c r="A1707" s="1">
+        <v>1705</v>
+      </c>
+      <c r="B1707" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1707">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:3">
+      <c r="A1708" s="1">
+        <v>1706</v>
+      </c>
+      <c r="B1708" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1708">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:3">
+      <c r="A1709" s="1">
+        <v>1707</v>
+      </c>
+      <c r="B1709" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1709">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:3">
+      <c r="A1710" s="1">
+        <v>1708</v>
+      </c>
+      <c r="B1710" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1710">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:3">
+      <c r="A1711" s="1">
+        <v>1709</v>
+      </c>
+      <c r="B1711" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1711">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:3">
+      <c r="A1712" s="1">
+        <v>1710</v>
+      </c>
+      <c r="B1712" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1712">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:3">
+      <c r="A1713" s="1">
+        <v>1711</v>
+      </c>
+      <c r="B1713" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1713">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:3">
+      <c r="A1714" s="1">
+        <v>1712</v>
+      </c>
+      <c r="B1714" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1714">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:3">
+      <c r="A1715" s="1">
+        <v>1713</v>
+      </c>
+      <c r="B1715" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1715">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:3">
+      <c r="A1716" s="1">
+        <v>1714</v>
+      </c>
+      <c r="B1716" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1716">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:3">
+      <c r="A1717" s="1">
+        <v>1715</v>
+      </c>
+      <c r="B1717" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1717">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:3">
+      <c r="A1718" s="1">
+        <v>1716</v>
+      </c>
+      <c r="B1718" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1718">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:3">
+      <c r="A1719" s="1">
+        <v>1717</v>
+      </c>
+      <c r="B1719" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1719">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:3">
+      <c r="A1720" s="1">
+        <v>1718</v>
+      </c>
+      <c r="B1720" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1720">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:3">
+      <c r="A1721" s="1">
+        <v>1719</v>
+      </c>
+      <c r="B1721" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1721">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:3">
+      <c r="A1722" s="1">
+        <v>1720</v>
+      </c>
+      <c r="B1722" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1722">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:3">
+      <c r="A1723" s="1">
+        <v>1721</v>
+      </c>
+      <c r="B1723" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1723">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:3">
+      <c r="A1724" s="1">
+        <v>1722</v>
+      </c>
+      <c r="B1724" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1724">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:3">
+      <c r="A1725" s="1">
+        <v>1723</v>
+      </c>
+      <c r="B1725" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1725">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:3">
+      <c r="A1726" s="1">
+        <v>1724</v>
+      </c>
+      <c r="B1726" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1726">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:3">
+      <c r="A1727" s="1">
+        <v>1725</v>
+      </c>
+      <c r="B1727" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1727">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:3">
+      <c r="A1728" s="1">
+        <v>1726</v>
+      </c>
+      <c r="B1728" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1728">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:3">
+      <c r="A1729" s="1">
+        <v>1727</v>
+      </c>
+      <c r="B1729" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1729">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:3">
+      <c r="A1730" s="1">
+        <v>1728</v>
+      </c>
+      <c r="B1730" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1730">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:3">
+      <c r="A1731" s="1">
+        <v>1729</v>
+      </c>
+      <c r="B1731" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1731">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:3">
+      <c r="A1732" s="1">
+        <v>1730</v>
+      </c>
+      <c r="B1732" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1732">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:3">
+      <c r="A1733" s="1">
+        <v>1731</v>
+      </c>
+      <c r="B1733" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1733">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:3">
+      <c r="A1734" s="1">
+        <v>1732</v>
+      </c>
+      <c r="B1734" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1734">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:3">
+      <c r="A1735" s="1">
+        <v>1733</v>
+      </c>
+      <c r="B1735" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1735">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:3">
+      <c r="A1736" s="1">
+        <v>1734</v>
+      </c>
+      <c r="B1736" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1736">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:3">
+      <c r="A1737" s="1">
+        <v>1735</v>
+      </c>
+      <c r="B1737" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1737">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:3">
+      <c r="A1738" s="1">
+        <v>1736</v>
+      </c>
+      <c r="B1738" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1738">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:3">
+      <c r="A1739" s="1">
+        <v>1737</v>
+      </c>
+      <c r="B1739" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1739">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:3">
+      <c r="A1740" s="1">
+        <v>1738</v>
+      </c>
+      <c r="B1740" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1740">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:3">
+      <c r="A1741" s="1">
+        <v>1739</v>
+      </c>
+      <c r="B1741" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1741">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:3">
+      <c r="A1742" s="1">
+        <v>1740</v>
+      </c>
+      <c r="B1742" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1742">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:3">
+      <c r="A1743" s="1">
+        <v>1741</v>
+      </c>
+      <c r="B1743" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1743">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:3">
+      <c r="A1744" s="1">
+        <v>1742</v>
+      </c>
+      <c r="B1744" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1744">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:3">
+      <c r="A1745" s="1">
+        <v>1743</v>
+      </c>
+      <c r="B1745" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1745">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:3">
+      <c r="A1746" s="1">
+        <v>1744</v>
+      </c>
+      <c r="B1746" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1746">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:3">
+      <c r="A1747" s="1">
+        <v>1745</v>
+      </c>
+      <c r="B1747" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1747">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:3">
+      <c r="A1748" s="1">
+        <v>1746</v>
+      </c>
+      <c r="B1748" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1748">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:3">
+      <c r="A1749" s="1">
+        <v>1747</v>
+      </c>
+      <c r="B1749" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1749">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:3">
+      <c r="A1750" s="1">
+        <v>1748</v>
+      </c>
+      <c r="B1750" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1750">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:3">
+      <c r="A1751" s="1">
+        <v>1749</v>
+      </c>
+      <c r="B1751" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1751">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:3">
+      <c r="A1752" s="1">
+        <v>1750</v>
+      </c>
+      <c r="B1752" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1752">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:3">
+      <c r="A1753" s="1">
+        <v>1751</v>
+      </c>
+      <c r="B1753" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1753">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:3">
+      <c r="A1754" s="1">
+        <v>1752</v>
+      </c>
+      <c r="B1754" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1754">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:3">
+      <c r="A1755" s="1">
+        <v>1753</v>
+      </c>
+      <c r="B1755" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1755">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:3">
+      <c r="A1756" s="1">
+        <v>1754</v>
+      </c>
+      <c r="B1756" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1756">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:3">
+      <c r="A1757" s="1">
+        <v>1755</v>
+      </c>
+      <c r="B1757" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1757">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:3">
+      <c r="A1758" s="1">
+        <v>1756</v>
+      </c>
+      <c r="B1758" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1758">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:3">
+      <c r="A1759" s="1">
+        <v>1757</v>
+      </c>
+      <c r="B1759" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1759">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:3">
+      <c r="A1760" s="1">
+        <v>1758</v>
+      </c>
+      <c r="B1760" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1760">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:3">
+      <c r="A1761" s="1">
+        <v>1759</v>
+      </c>
+      <c r="B1761" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1761">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:3">
+      <c r="A1762" s="1">
+        <v>1760</v>
+      </c>
+      <c r="B1762" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1762">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:3">
+      <c r="A1763" s="1">
+        <v>1761</v>
+      </c>
+      <c r="B1763" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1763">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:3">
+      <c r="A1764" s="1">
+        <v>1762</v>
+      </c>
+      <c r="B1764" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1764">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:3">
+      <c r="A1765" s="1">
+        <v>1763</v>
+      </c>
+      <c r="B1765" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1765">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:3">
+      <c r="A1766" s="1">
+        <v>1764</v>
+      </c>
+      <c r="B1766" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1766">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:3">
+      <c r="A1767" s="1">
+        <v>1765</v>
+      </c>
+      <c r="B1767" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1767">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:3">
+      <c r="A1768" s="1">
+        <v>1766</v>
+      </c>
+      <c r="B1768" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1768">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:3">
+      <c r="A1769" s="1">
+        <v>1767</v>
+      </c>
+      <c r="B1769" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1769">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:3">
+      <c r="A1770" s="1">
+        <v>1768</v>
+      </c>
+      <c r="B1770" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1770">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:3">
+      <c r="A1771" s="1">
+        <v>1769</v>
+      </c>
+      <c r="B1771" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1771">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:3">
+      <c r="A1772" s="1">
+        <v>1770</v>
+      </c>
+      <c r="B1772" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1772">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:3">
+      <c r="A1773" s="1">
+        <v>1771</v>
+      </c>
+      <c r="B1773" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1773">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:3">
+      <c r="A1774" s="1">
+        <v>1772</v>
+      </c>
+      <c r="B1774" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1774">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:3">
+      <c r="A1775" s="1">
+        <v>1773</v>
+      </c>
+      <c r="B1775" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1775">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:3">
+      <c r="A1776" s="1">
+        <v>1774</v>
+      </c>
+      <c r="B1776" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1776">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:3">
+      <c r="A1777" s="1">
+        <v>1775</v>
+      </c>
+      <c r="B1777" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1777">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:3">
+      <c r="A1778" s="1">
+        <v>1776</v>
+      </c>
+      <c r="B1778" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1778">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:3">
+      <c r="A1779" s="1">
+        <v>1777</v>
+      </c>
+      <c r="B1779" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1779">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:3">
+      <c r="A1780" s="1">
+        <v>1778</v>
+      </c>
+      <c r="B1780" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1780">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:3">
+      <c r="A1781" s="1">
+        <v>1779</v>
+      </c>
+      <c r="B1781" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1781">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:3">
+      <c r="A1782" s="1">
+        <v>1780</v>
+      </c>
+      <c r="B1782" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1782">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:3">
+      <c r="A1783" s="1">
+        <v>1781</v>
+      </c>
+      <c r="B1783" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1783">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:3">
+      <c r="A1784" s="1">
+        <v>1782</v>
+      </c>
+      <c r="B1784" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1784">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:3">
+      <c r="A1785" s="1">
+        <v>1783</v>
+      </c>
+      <c r="B1785" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1785">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:3">
+      <c r="A1786" s="1">
+        <v>1784</v>
+      </c>
+      <c r="B1786" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1786">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:3">
+      <c r="A1787" s="1">
+        <v>1785</v>
+      </c>
+      <c r="B1787" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1787">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:3">
+      <c r="A1788" s="1">
+        <v>1786</v>
+      </c>
+      <c r="B1788" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1788">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:3">
+      <c r="A1789" s="1">
+        <v>1787</v>
+      </c>
+      <c r="B1789" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1789">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:3">
+      <c r="A1790" s="1">
+        <v>1788</v>
+      </c>
+      <c r="B1790" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1790">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:3">
+      <c r="A1791" s="1">
+        <v>1789</v>
+      </c>
+      <c r="B1791" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1791">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:3">
+      <c r="A1792" s="1">
+        <v>1790</v>
+      </c>
+      <c r="B1792" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1792">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:3">
+      <c r="A1793" s="1">
+        <v>1791</v>
+      </c>
+      <c r="B1793" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1793">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:3">
+      <c r="A1794" s="1">
+        <v>1792</v>
+      </c>
+      <c r="B1794" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1794">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:3">
+      <c r="A1795" s="1">
+        <v>1793</v>
+      </c>
+      <c r="B1795" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1795">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:3">
+      <c r="A1796" s="1">
+        <v>1794</v>
+      </c>
+      <c r="B1796" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1796">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:3">
+      <c r="A1797" s="1">
+        <v>1795</v>
+      </c>
+      <c r="B1797" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1797">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:3">
+      <c r="A1798" s="1">
+        <v>1796</v>
+      </c>
+      <c r="B1798" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1798">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:3">
+      <c r="A1799" s="1">
+        <v>1797</v>
+      </c>
+      <c r="B1799" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1799">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:3">
+      <c r="A1800" s="1">
+        <v>1798</v>
+      </c>
+      <c r="B1800" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1800">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:3">
+      <c r="A1801" s="1">
+        <v>1799</v>
+      </c>
+      <c r="B1801" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1801">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:3">
+      <c r="A1802" s="1">
+        <v>1800</v>
+      </c>
+      <c r="B1802" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1802">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:3">
+      <c r="A1803" s="1">
+        <v>1801</v>
+      </c>
+      <c r="B1803" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1803">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:3">
+      <c r="A1804" s="1">
+        <v>1802</v>
+      </c>
+      <c r="B1804" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1804">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:3">
+      <c r="A1805" s="1">
+        <v>1803</v>
+      </c>
+      <c r="B1805" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1805">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:3">
+      <c r="A1806" s="1">
+        <v>1804</v>
+      </c>
+      <c r="B1806" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1806">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:3">
+      <c r="A1807" s="1">
+        <v>1805</v>
+      </c>
+      <c r="B1807" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1807">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:3">
+      <c r="A1808" s="1">
+        <v>1806</v>
+      </c>
+      <c r="B1808" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1808">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:3">
+      <c r="A1809" s="1">
+        <v>1807</v>
+      </c>
+      <c r="B1809" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1809">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:3">
+      <c r="A1810" s="1">
+        <v>1808</v>
+      </c>
+      <c r="B1810" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1810">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:3">
+      <c r="A1811" s="1">
+        <v>1809</v>
+      </c>
+      <c r="B1811" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1811">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:3">
+      <c r="A1812" s="1">
+        <v>1810</v>
+      </c>
+      <c r="B1812" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1812">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:3">
+      <c r="A1813" s="1">
+        <v>1811</v>
+      </c>
+      <c r="B1813" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1813">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:3">
+      <c r="A1814" s="1">
+        <v>1812</v>
+      </c>
+      <c r="B1814" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1814">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:3">
+      <c r="A1815" s="1">
+        <v>1813</v>
+      </c>
+      <c r="B1815" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1815">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:3">
+      <c r="A1816" s="1">
+        <v>1814</v>
+      </c>
+      <c r="B1816" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1816">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:3">
+      <c r="A1817" s="1">
+        <v>1815</v>
+      </c>
+      <c r="B1817" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1817">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:3">
+      <c r="A1818" s="1">
+        <v>1816</v>
+      </c>
+      <c r="B1818" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1818">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:3">
+      <c r="A1819" s="1">
+        <v>1817</v>
+      </c>
+      <c r="B1819" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1819">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:3">
+      <c r="A1820" s="1">
+        <v>1818</v>
+      </c>
+      <c r="B1820" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1820">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:3">
+      <c r="A1821" s="1">
+        <v>1819</v>
+      </c>
+      <c r="B1821" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1821">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:3">
+      <c r="A1822" s="1">
+        <v>1820</v>
+      </c>
+      <c r="B1822" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1822">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:3">
+      <c r="A1823" s="1">
+        <v>1821</v>
+      </c>
+      <c r="B1823" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1823">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:3">
+      <c r="A1824" s="1">
+        <v>1822</v>
+      </c>
+      <c r="B1824" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1824">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:3">
+      <c r="A1825" s="1">
+        <v>1823</v>
+      </c>
+      <c r="B1825" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1825">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:3">
+      <c r="A1826" s="1">
+        <v>1824</v>
+      </c>
+      <c r="B1826" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1826">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:3">
+      <c r="A1827" s="1">
+        <v>1825</v>
+      </c>
+      <c r="B1827" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1827">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:3">
+      <c r="A1828" s="1">
+        <v>1826</v>
+      </c>
+      <c r="B1828" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1828">
+        <v>93.03</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:3">
+      <c r="A1829" s="1">
+        <v>1827</v>
+      </c>
+      <c r="B1829" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1829">
+        <v>93.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>